<commit_message>
merge with 2nd line's content
</commit_message>
<xml_diff>
--- a/shCDP1.xlsx
+++ b/shCDP1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phe\Documents\tech\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0885353-772A-4DCC-970B-240C0205932A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B97AE0-2C12-48C3-BF23-67416A243D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="20850" windowHeight="11835" xr2:uid="{E0CE312C-0616-4794-AFD3-346D8F69FF7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19725" windowHeight="11760" xr2:uid="{E0CE312C-0616-4794-AFD3-346D8F69FF7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>index</t>
   </si>
@@ -53,33 +53,12 @@
     <t>ca1001sw2</t>
   </si>
   <si>
-    <t>nap2</t>
-  </si>
-  <si>
-    <t>nap3</t>
-  </si>
-  <si>
-    <t>g1/0/1</t>
-  </si>
-  <si>
     <t>g1/0/2</t>
   </si>
   <si>
-    <t>g1/0/7</t>
-  </si>
-  <si>
-    <t>g1/0/8</t>
-  </si>
-  <si>
-    <t>SEPnsw1</t>
-  </si>
-  <si>
     <t>SEPnsw2</t>
   </si>
   <si>
-    <t>SEPnap1</t>
-  </si>
-  <si>
     <t>ca1001</t>
   </si>
   <si>
@@ -101,13 +80,10 @@
     <t>g1/0/48</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>nan</t>
+    <t>nnn</t>
+  </si>
+  <si>
+    <t>mmm</t>
   </si>
 </sst>
 </file>
@@ -459,18 +435,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1D43F3-8CB5-4A38-8FC6-DB62D4E579CD}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D8"/>
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,156 +454,90 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>